<commit_message>
Comments from Kamal and Sayan Added
</commit_message>
<xml_diff>
--- a/data_dict_reduced.xlsx
+++ b/data_dict_reduced.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Infosys Limited\Data Science Workspace\upgrad\Course2_GroupProject1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="137">
   <si>
     <t>LoanStatNew</t>
   </si>
@@ -22,9 +27,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>data_type</t>
-  </si>
-  <si>
     <t>addr_state</t>
   </si>
   <si>
@@ -368,13 +370,86 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Type of analysis required</t>
+  </si>
+  <si>
+    <t>Sayan's Comments</t>
+  </si>
+  <si>
+    <t>Remove column</t>
+  </si>
+  <si>
+    <t>Free Text</t>
+  </si>
+  <si>
+    <t>Check for number of unique values. Possibly need removal</t>
+  </si>
+  <si>
+    <t>Need to remove %</t>
+  </si>
+  <si>
+    <t>I believe, we should remove rows that are current from analysis and then at the end we might use our analysis on the ongoing to loans to indicate risky ones.</t>
+  </si>
+  <si>
+    <t>histogram
+box plot
+box plot segmented by loan_status</t>
+  </si>
+  <si>
+    <t>Is there a relation between this and open_acc? Can we derive any new variable from these two?</t>
+  </si>
+  <si>
+    <t>rank-frequency plot
+grouped bar chart by loan status</t>
+  </si>
+  <si>
+    <t>histogram
+box plot
+Violin plot
+box plot segmented by loan_status</t>
+  </si>
+  <si>
+    <t>Need to remove months</t>
+  </si>
+  <si>
+    <t>ratio</t>
+  </si>
+  <si>
+    <t>Need more understanding of this data.
+Can we derive new variable as percentage of total loan amount?</t>
+  </si>
+  <si>
+    <t>histogram
+box plot
+Violin plot
+box plot segmented by loan_status
+Correlation</t>
+  </si>
+  <si>
+    <t>Ordinal</t>
+  </si>
+  <si>
+    <t>Bar chart
+grouped bar chart by loan status</t>
+  </si>
+  <si>
+    <t>Basic data_type</t>
+  </si>
+  <si>
+    <t>It is likely to be correlated with principle and loan amount, still can include in pair plot/ corrplot
+Additionally we can derive new variable as percentage of total loan amount. Then analyze that in similar way</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1202,21 +1277,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14:I25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K46" sqref="I1:K1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1224,10 +1299,13 @@
     <col min="4" max="5" width="11.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="43.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="45.75" customHeight="1">
+    <row r="1" spans="1:11" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1236,1048 +1314,1349 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="30">
+      <c r="J1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30">
+        <v>111</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30">
+        <v>111</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="45">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30">
+        <v>111</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="60">
+        <v>111</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>16</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30">
+        <v>111</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45">
+        <v>111</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>19</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30">
+        <v>111</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>20</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30">
+        <v>111</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>23</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30">
+        <v>111</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30">
+        <v>111</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D13" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="45">
+        <v>111</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+        <v>107</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30">
+        <v>107</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>32</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30">
+        <v>107</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>33</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30">
+        <v>107</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>34</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30">
+        <v>107</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>35</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30">
+        <v>107</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+    </row>
+    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>36</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>107</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>39</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="D21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="30">
+        <v>107</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>40</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="D22" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="60">
+        <v>107</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>41</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="30">
+        <v>107</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>42</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+        <v>107</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="D25" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="30">
+        <v>107</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>50</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="D26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+        <v>112</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>52</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="30">
+        <v>112</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+    </row>
+    <row r="28" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>58</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="30">
+        <v>112</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>73</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="D29" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>112</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>80</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="D30" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="30">
+        <v>112</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>81</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="D31" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>112</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>85</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="D32" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>112</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>86</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="30">
+        <v>112</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>87</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>112</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>89</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>112</v>
+      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>90</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="D36" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" ht="45">
+      <c r="I36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>91</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="D37" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30">
+        <v>106</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>92</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="30">
+        <v>106</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>94</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="30">
+        <v>106</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>95</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="D40" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="30">
+        <v>106</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="J40" s="5"/>
+      <c r="K40" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>99</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
+        <v>106</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>105</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="D42" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="30">
+        <v>106</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="K42" s="5"/>
+    </row>
+    <row r="43" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>106</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>106</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J43" s="5"/>
+      <c r="K43" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>107</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
+        <v>106</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>108</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="D45" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
+        <v>106</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="K45" s="5"/>
+    </row>
+    <row r="46" spans="1:11" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>109</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="D46" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="45">
+        <v>106</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>111</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="D47" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" ht="30">
+      <c r="H47" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>112</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="D48" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="30">
+        <v>106</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="K48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>114</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2" t="s">
-        <v>107</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="K49" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
includes ashutosh's updates by peeyush
</commit_message>
<xml_diff>
--- a/data_dict_reduced.xlsx
+++ b/data_dict_reduced.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="158">
   <si>
     <t>LoanStatNew</t>
   </si>
@@ -497,6 +497,46 @@
   <si>
     <t>histogram
 box plot</t>
+  </si>
+  <si>
+    <t>histogram
+box plot
+Correleation with Loan Status
+bivariate analysis too</t>
+  </si>
+  <si>
+    <t>derived matrix of collection_recovery_fee and recoveries can help us understand the percentage the recovery fee is to the total recovery</t>
+  </si>
+  <si>
+    <t>Date / Interval</t>
+  </si>
+  <si>
+    <t>histogram
+box plot
+Correleation with Loan Status
+relation between when the loan was asked (column name?)</t>
+  </si>
+  <si>
+    <t>Can be used to check if the loan status viz a viz a particular ogranisation is more or not. Is there are racket</t>
+  </si>
+  <si>
+    <t>histogram
+box plot
+Correleation with Loan Status
+bivariate analysis too with funded_amnt_inv
+derived matrix funded_amnt_inv/funded_amnt</t>
+  </si>
+  <si>
+    <t>histogram
+box plot
+Correleation with Loan Status
+bivariate analysis too with funded_amnt
+derived matrix funded_amnt_inv/funded_amnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relation with Loan Status
+and other params
+</t>
   </si>
 </sst>
 </file>
@@ -1350,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,11 +1462,15 @@
         <v>111</v>
       </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I2" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>4</v>
       </c>
@@ -1447,11 +1491,15 @@
         <v>111</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="I3" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>11</v>
       </c>
@@ -1472,13 +1520,17 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="I4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="K4" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>13</v>
       </c>
@@ -1499,8 +1551,12 @@
         <v>111</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="I5" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -1553,11 +1609,15 @@
         <v>111</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="I7" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>18</v>
       </c>
@@ -1578,11 +1638,15 @@
         <v>111</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="I8" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>153</v>
+      </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>19</v>
       </c>
@@ -1603,11 +1667,15 @@
         <v>111</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="I9" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>150</v>
+      </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>20</v>
       </c>
@@ -1628,11 +1696,15 @@
         <v>111</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="I10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>154</v>
+      </c>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>23</v>
       </c>
@@ -1653,11 +1725,15 @@
         <v>111</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="I11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>155</v>
+      </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>24</v>
       </c>
@@ -1678,11 +1754,15 @@
         <v>111</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="I12" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>156</v>
+      </c>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>25</v>
       </c>
@@ -1703,10 +1783,12 @@
         <v>111</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J13" s="2"/>
+      <c r="I13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>157</v>
+      </c>
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -2773,7 +2855,6 @@
       <c r="K49" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K49"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Included - H/M/L and derived matrix usability
</commit_message>
<xml_diff>
--- a/data_dict_reduced.xlsx
+++ b/data_dict_reduced.xlsx
@@ -15,14 +15,14 @@
     <sheet name="data_dict_reduced" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_dict_reduced!$A$1:$K$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data_dict_reduced!$A$1:$M$49</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="165">
   <si>
     <t>LoanStatNew</t>
   </si>
@@ -537,6 +537,27 @@
     <t xml:space="preserve">relation with Loan Status
 and other params
 </t>
+  </si>
+  <si>
+    <t>Importance ( H, M, L)</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Useful for derived matrix</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -1388,10 +1409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1402,13 +1423,15 @@
     <col min="4" max="5" width="11.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="43.140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="43.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1432,16 +1455,22 @@
         <v>116</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2</v>
       </c>
@@ -1462,15 +1491,21 @@
         <v>111</v>
       </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>4</v>
       </c>
@@ -1491,15 +1526,21 @@
         <v>111</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>11</v>
       </c>
@@ -1520,17 +1561,23 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>13</v>
       </c>
@@ -1551,15 +1598,21 @@
         <v>111</v>
       </c>
       <c r="H5" s="2"/>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="L5" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>15</v>
       </c>
@@ -1580,15 +1633,21 @@
       <c r="H6" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5"/>
+      <c r="M6" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>16</v>
       </c>
@@ -1609,15 +1668,21 @@
         <v>111</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K7" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>18</v>
       </c>
@@ -1638,15 +1703,21 @@
         <v>111</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K8" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="L8" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>19</v>
       </c>
@@ -1667,15 +1738,21 @@
         <v>111</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="L9" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>20</v>
       </c>
@@ -1696,15 +1773,21 @@
         <v>111</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="L10" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>23</v>
       </c>
@@ -1725,15 +1808,21 @@
         <v>111</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="L11" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>24</v>
       </c>
@@ -1754,15 +1843,21 @@
         <v>111</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="L12" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>25</v>
       </c>
@@ -1783,15 +1878,21 @@
         <v>111</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K13" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="L13" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="K13" s="2"/>
-    </row>
-    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>26</v>
       </c>
@@ -1814,11 +1915,17 @@
       <c r="H14" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="K14" s="2"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>27</v>
       </c>
@@ -1841,11 +1948,17 @@
       <c r="H15" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="K15" s="2"/>
-    </row>
-    <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>32</v>
       </c>
@@ -1868,11 +1981,17 @@
       <c r="H16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>33</v>
       </c>
@@ -1895,11 +2014,17 @@
       <c r="H17" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>34</v>
       </c>
@@ -1922,13 +2047,19 @@
       <c r="H18" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2" t="s">
+      <c r="I18" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>35</v>
       </c>
@@ -1951,11 +2082,17 @@
       <c r="H19" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>36</v>
       </c>
@@ -1976,11 +2113,17 @@
         <v>107</v>
       </c>
       <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="I20" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>39</v>
       </c>
@@ -2001,11 +2144,17 @@
         <v>107</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="K21" s="2"/>
-    </row>
-    <row r="22" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>40</v>
       </c>
@@ -2026,11 +2175,17 @@
         <v>107</v>
       </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
+      <c r="I22" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="K22" s="2"/>
-    </row>
-    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>41</v>
       </c>
@@ -2051,11 +2206,17 @@
         <v>107</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="I23" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>164</v>
+      </c>
       <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>42</v>
       </c>
@@ -2079,14 +2240,20 @@
         <v>115</v>
       </c>
       <c r="I24" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K24" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2" t="s">
+      <c r="L24" s="2"/>
+      <c r="M24" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44</v>
       </c>
@@ -2109,11 +2276,17 @@
       <c r="H25" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="I25" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>50</v>
       </c>
@@ -2133,17 +2306,23 @@
       <c r="G26" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K26" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J26" s="6" t="s">
+      <c r="L26" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="K26" s="6" t="s">
+      <c r="M26" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>52</v>
       </c>
@@ -2164,17 +2343,23 @@
         <v>112</v>
       </c>
       <c r="H27" s="2"/>
-      <c r="I27" s="6" t="s">
+      <c r="I27" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K27" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J27" s="6" t="s">
+      <c r="L27" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="K27" s="6" t="s">
+      <c r="M27" s="6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>58</v>
       </c>
@@ -2195,15 +2380,21 @@
         <v>112</v>
       </c>
       <c r="H28" s="2"/>
-      <c r="I28" s="6" t="s">
+      <c r="I28" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K28" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="J28" s="6"/>
-      <c r="K28" s="6" t="s">
+      <c r="L28" s="6"/>
+      <c r="M28" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>73</v>
       </c>
@@ -2224,17 +2415,23 @@
         <v>112</v>
       </c>
       <c r="H29" s="2"/>
-      <c r="I29" s="6" t="s">
+      <c r="I29" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K29" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="J29" s="6" t="s">
+      <c r="L29" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="M29" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>80</v>
       </c>
@@ -2255,17 +2452,23 @@
         <v>112</v>
       </c>
       <c r="H30" s="2"/>
-      <c r="I30" s="6" t="s">
+      <c r="I30" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K30" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J30" s="6" t="s">
+      <c r="L30" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="K30" s="6" t="s">
+      <c r="M30" s="6" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>81</v>
       </c>
@@ -2286,17 +2489,23 @@
         <v>112</v>
       </c>
       <c r="H31" s="2"/>
-      <c r="I31" s="6" t="s">
+      <c r="I31" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K31" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J31" s="6" t="s">
+      <c r="L31" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="K31" s="6" t="s">
+      <c r="M31" s="6" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>85</v>
       </c>
@@ -2317,15 +2526,21 @@
         <v>112</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="I32" s="6" t="s">
+      <c r="I32" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K32" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="L32" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="K32" s="2"/>
-    </row>
-    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="M32" s="2"/>
+    </row>
+    <row r="33" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>86</v>
       </c>
@@ -2346,15 +2561,21 @@
         <v>112</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="I33" s="6" t="s">
+      <c r="I33" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K33" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J33" s="6" t="s">
+      <c r="L33" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="M33" s="2"/>
+    </row>
+    <row r="34" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>87</v>
       </c>
@@ -2375,15 +2596,21 @@
         <v>112</v>
       </c>
       <c r="H34" s="2"/>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K34" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="J34" s="6" t="s">
+      <c r="L34" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="K34" s="2"/>
-    </row>
-    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="M34" s="2"/>
+    </row>
+    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>89</v>
       </c>
@@ -2404,17 +2631,23 @@
         <v>112</v>
       </c>
       <c r="H35" s="2"/>
-      <c r="I35" s="6" t="s">
+      <c r="I35" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K35" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="L35" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="K35" s="6" t="s">
+      <c r="M35" s="6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>90</v>
       </c>
@@ -2438,16 +2671,22 @@
         <v>113</v>
       </c>
       <c r="I36" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="J36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="M36" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>91</v>
       </c>
@@ -2470,17 +2709,23 @@
       <c r="H37" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I37" s="5" t="s">
+      <c r="I37" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K37" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="J37" s="5" t="s">
+      <c r="L37" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="M37" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>92</v>
       </c>
@@ -2503,15 +2748,21 @@
       <c r="H38" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I38" s="5" t="s">
+      <c r="I38" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K38" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J38" s="5" t="s">
+      <c r="L38" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="K38" s="5"/>
-    </row>
-    <row r="39" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M38" s="5"/>
+    </row>
+    <row r="39" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>94</v>
       </c>
@@ -2534,17 +2785,23 @@
       <c r="H39" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="I39" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K39" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="L39" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="M39" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>95</v>
       </c>
@@ -2567,15 +2824,21 @@
       <c r="H40" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I40" s="5" t="s">
+      <c r="I40" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K40" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="J40" s="5"/>
-      <c r="K40" s="5" t="s">
+      <c r="L40" s="5"/>
+      <c r="M40" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>99</v>
       </c>
@@ -2598,15 +2861,21 @@
       <c r="H41" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I41" s="5" t="s">
+      <c r="I41" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K41" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="J41" s="5" t="s">
+      <c r="L41" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="K41" s="5"/>
-    </row>
-    <row r="42" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="M41" s="5"/>
+    </row>
+    <row r="42" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>105</v>
       </c>
@@ -2629,15 +2898,21 @@
       <c r="H42" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I42" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K42" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="J42" s="5" t="s">
+      <c r="L42" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="K42" s="5"/>
-    </row>
-    <row r="43" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="M42" s="5"/>
+    </row>
+    <row r="43" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>106</v>
       </c>
@@ -2660,15 +2935,21 @@
       <c r="H43" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="I43" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K43" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="J43" s="5"/>
-      <c r="K43" s="5" t="s">
+      <c r="L43" s="5"/>
+      <c r="M43" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>107</v>
       </c>
@@ -2691,17 +2972,23 @@
       <c r="H44" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="I44" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K44" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="J44" s="5" t="s">
+      <c r="L44" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K44" s="5" t="s">
+      <c r="M44" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>108</v>
       </c>
@@ -2724,15 +3011,21 @@
       <c r="H45" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I45" s="5" t="s">
+      <c r="I45" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K45" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="J45" s="5" t="s">
+      <c r="L45" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="K45" s="5"/>
-    </row>
-    <row r="46" spans="1:11" ht="135" x14ac:dyDescent="0.25">
+      <c r="M45" s="5"/>
+    </row>
+    <row r="46" spans="1:13" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>109</v>
       </c>
@@ -2755,17 +3048,23 @@
       <c r="H46" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I46" s="5" t="s">
+      <c r="I46" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K46" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="J46" s="5" t="s">
+      <c r="L46" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="K46" s="5" t="s">
+      <c r="M46" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>111</v>
       </c>
@@ -2786,13 +3085,19 @@
       <c r="H47" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="5" t="s">
+      <c r="I47" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>112</v>
       </c>
@@ -2815,15 +3120,21 @@
       <c r="H48" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I48" s="5" t="s">
+      <c r="I48" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K48" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="J48" s="5" t="s">
+      <c r="L48" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="K48" s="5"/>
-    </row>
-    <row r="49" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="M48" s="5"/>
+    </row>
+    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>114</v>
       </c>
@@ -2846,13 +3157,19 @@
       <c r="H49" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I49" s="5" t="s">
+      <c r="I49" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="K49" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J49" s="5" t="s">
+      <c r="L49" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="K49" s="5"/>
+      <c r="M49" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Sayan's comment on H/M/L and missing values
</commit_message>
<xml_diff>
--- a/data_dict_reduced.xlsx
+++ b/data_dict_reduced.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peeyush_singhal\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Infosys Limited\Data Science Workspace\upgrad\Course2_GroupProject1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="data_dict_reduced" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="197">
   <si>
     <t>LoanStatNew</t>
   </si>
@@ -421,10 +421,6 @@
   </si>
   <si>
     <t>ratio</t>
-  </si>
-  <si>
-    <t>Need more understanding of this data.
-Can we derive new variable as percentage of total loan amount?</t>
   </si>
   <si>
     <t>histogram
@@ -444,23 +440,11 @@
     <t>Basic data_type</t>
   </si>
   <si>
-    <t>It is likely to be correlated with principle and loan amount, still can include in pair plot/ corrplot
-Additionally we can derive new variable as percentage of total loan amount. Then analyze that in similar way</t>
-  </si>
-  <si>
     <t xml:space="preserve">histogram
 box plot
 </t>
   </si>
   <si>
-    <t xml:space="preserve">This data has lot of NA values
-This directly have relationship with customer being deliquent </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This data has lot of NA values
-</t>
-  </si>
-  <si>
     <t>histogram
 box plot
 Correleation with Loan Status</t>
@@ -472,9 +456,6 @@
     <t>This data has only 16 Jun and 16 July as date and that too for Current Customers. I thinks we can delete this column from analysis</t>
   </si>
   <si>
-    <t>This data only has NA, we can delete it from our analysis</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -486,9 +467,6 @@
     <t xml:space="preserve">histogram
 box plot
 bivariate analysis with loan_Status </t>
-  </si>
-  <si>
-    <t>Values only available for charged off customers.</t>
   </si>
   <si>
     <t>loan status vs purpose
@@ -539,31 +517,153 @@
 </t>
   </si>
   <si>
+    <t>Has missing value?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Yes - loan amount as pct of annual income</t>
+  </si>
+  <si>
+    <t>Not required</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Yes, &gt;2000</t>
+  </si>
+  <si>
+    <t>Yes, ~1000</t>
+  </si>
+  <si>
+    <t>Remove column - this will not be avilable for new customers</t>
+  </si>
+  <si>
+    <t>This data has lot of NA values
+This directly have relationship with customer being deliquent.
+Remove Column - this will not be available for new customer</t>
+  </si>
+  <si>
+    <t>Yes - proportion of loan amount</t>
+  </si>
+  <si>
+    <t>Can we delete this column? This information will not be available for new customer</t>
+  </si>
+  <si>
+    <t>Yes - yearly installment proportion to annual income</t>
+  </si>
+  <si>
+    <t>Can we delete this column?</t>
+  </si>
+  <si>
+    <t>Yes, 2</t>
+  </si>
+  <si>
+    <t>Will this information be available for new customer</t>
+  </si>
+  <si>
+    <t>Yes - Proportion of installment</t>
+  </si>
+  <si>
+    <t>Yes, 71</t>
+  </si>
+  <si>
+    <t>Yes, mentioned in other columns</t>
+  </si>
+  <si>
+    <t>Yes, &gt;35k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This data has lot of NA values - can we impute with 0?
+</t>
+  </si>
+  <si>
+    <t>This data only has NA, we can delete it from our analysis - Is this right?</t>
+  </si>
+  <si>
+    <t>Yes, &lt;1k</t>
+  </si>
+  <si>
+    <t>Yes, proportion of public record</t>
+  </si>
+  <si>
+    <t>Can we impute 0?</t>
+  </si>
+  <si>
+    <t>Values only available for charged off customers. - should we delete this column?</t>
+  </si>
+  <si>
+    <t>Yes, 50</t>
+  </si>
+  <si>
+    <t>Need to remove %
+Can we impute using 0?</t>
+  </si>
+  <si>
+    <t>Yes - proportion of total account</t>
+  </si>
+  <si>
+    <t>Yes - mentioned in other column</t>
+  </si>
+  <si>
+    <t>Need more understanding of this data.
+Can we derive new variable as percentage of total loan amount?
+Will this information be available for new customer?</t>
+  </si>
+  <si>
+    <t>It is likely to be correlated with principle and loan amount, still can include in pair plot/ corrplot
+Additionally we can derive new variable as percentage of total loan amount. Then analyze that in similar way
+Will this information be available for new customer?</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Will this information be available for new customer?</t>
+  </si>
+  <si>
     <t>Importance ( H, M, L)</t>
   </si>
   <si>
+    <t>Useful for derived matrix</t>
+  </si>
+  <si>
     <t>L</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>H</t>
   </si>
   <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>M</t>
   </si>
   <si>
-    <t>Useful for derived matrix</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Y</t>
+    <t>Potential impact</t>
+  </si>
+  <si>
+    <t>use in derived metrics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -700,7 +800,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -889,6 +989,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1068,7 +1192,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1086,6 +1210,36 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1189,7 +1343,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1224,7 +1378,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1409,10 +1563,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="J11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,15 +1580,16 @@
     <col min="4" max="5" width="11.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="1"/>
+    <col min="8" max="11" width="9.140625" style="1"/>
     <col min="12" max="12" width="43.140625" style="1" customWidth="1"/>
     <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="14" width="10.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1440,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>104</v>
@@ -1455,13 +1613,13 @@
         <v>116</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="K1" s="3" t="s">
         <v>117</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="K1" s="16" t="s">
+        <v>189</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>118</v>
@@ -1469,8 +1627,17 @@
       <c r="M1" s="3" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N1" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2</v>
       </c>
@@ -1491,21 +1658,30 @@
         <v>111</v>
       </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>100</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>191</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>127</v>
       </c>
       <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="N2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>4</v>
       </c>
@@ -1526,128 +1702,152 @@
         <v>111</v>
       </c>
       <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>102</v>
       </c>
+      <c r="J3" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="L3" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="N3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K4" s="6" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="M4" s="2" t="s">
+      <c r="J4" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="M4" s="9" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+    </row>
+    <row r="5" spans="1:16" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
         <v>13</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K5" s="6" t="s">
+      <c r="H5" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="I5" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="J5" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="1:16" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K6" s="5" t="s">
+      <c r="I6" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5" t="s">
+      <c r="J6" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>16</v>
       </c>
@@ -1668,21 +1868,30 @@
         <v>111</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>102</v>
       </c>
+      <c r="J7" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="L7" s="6" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="N7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>18</v>
       </c>
@@ -1703,21 +1912,30 @@
         <v>111</v>
       </c>
       <c r="H8" s="2"/>
-      <c r="I8" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>152</v>
+      <c r="I8" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>191</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="N8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>19</v>
       </c>
@@ -1738,21 +1956,30 @@
         <v>111</v>
       </c>
       <c r="H9" s="2"/>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="M9" s="2"/>
-    </row>
-    <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="O9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>20</v>
       </c>
@@ -1773,21 +2000,32 @@
         <v>111</v>
       </c>
       <c r="H10" s="2"/>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="M10" s="2"/>
-    </row>
-    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="P10" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>23</v>
       </c>
@@ -1808,21 +2046,30 @@
         <v>111</v>
       </c>
       <c r="H11" s="2"/>
-      <c r="I11" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J11" s="2" t="s">
+      <c r="I11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>24</v>
       </c>
@@ -1843,21 +2090,30 @@
         <v>111</v>
       </c>
       <c r="H12" s="2"/>
-      <c r="I12" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>102</v>
       </c>
+      <c r="J12" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>191</v>
+      </c>
       <c r="L12" s="6" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N12" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>25</v>
       </c>
@@ -1878,21 +2134,30 @@
         <v>111</v>
       </c>
       <c r="H13" s="2"/>
-      <c r="I13" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>133</v>
+      <c r="I13" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K13" s="15" t="s">
+        <v>193</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N13" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>26</v>
       </c>
@@ -1915,50 +2180,62 @@
       <c r="H14" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="N14" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
         <v>27</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="5" t="s">
+      <c r="F15" s="7"/>
+      <c r="G15" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="I15" s="7"/>
+      <c r="J15" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+    </row>
+    <row r="16" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>32</v>
       </c>
@@ -1981,17 +2258,24 @@
       <c r="H16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K16" s="15" t="s">
+        <v>191</v>
+      </c>
       <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M16" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>33</v>
       </c>
@@ -2014,17 +2298,26 @@
       <c r="H17" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K17" s="15" t="s">
+        <v>191</v>
+      </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N17" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>34</v>
       </c>
@@ -2047,19 +2340,28 @@
       <c r="H18" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K18" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N18" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>35</v>
       </c>
@@ -2082,17 +2384,26 @@
       <c r="H19" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>191</v>
+      </c>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N19" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>36</v>
       </c>
@@ -2113,17 +2424,28 @@
         <v>107</v>
       </c>
       <c r="H20" s="2"/>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="2"/>
+      <c r="J20" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="N20" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="O20" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P20" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>39</v>
       </c>
@@ -2144,17 +2466,28 @@
         <v>107</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>191</v>
+      </c>
       <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="M21" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>40</v>
       </c>
@@ -2175,17 +2508,24 @@
         <v>107</v>
       </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>191</v>
+      </c>
       <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="M22" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="N22" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+    </row>
+    <row r="23" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>41</v>
       </c>
@@ -2206,17 +2546,26 @@
         <v>107</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="N23" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>42</v>
       </c>
@@ -2240,89 +2589,101 @@
         <v>115</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K24" s="2" t="s">
         <v>100</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>193</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="N24" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>44</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="G25" s="5" t="s">
+      <c r="F25" s="7"/>
+      <c r="G25" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J25" s="2" t="s">
+      <c r="I25" s="7"/>
+      <c r="J25" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+    </row>
+    <row r="26" spans="1:16" s="8" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>50</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="K26" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="M26" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>50</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="M26" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+    </row>
+    <row r="27" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>52</v>
       </c>
@@ -2343,169 +2704,196 @@
         <v>112</v>
       </c>
       <c r="H27" s="2"/>
-      <c r="I27" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K27" s="6" t="s">
+      <c r="I27" s="6" t="s">
         <v>102</v>
       </c>
+      <c r="J27" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>191</v>
+      </c>
       <c r="L27" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="N27" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" s="8" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>58</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="M27" s="6" t="s">
+      <c r="J28" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+    </row>
+    <row r="29" spans="1:16" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>73</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>58</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="J29" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K29" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="P29" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" s="8" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>80</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2" t="s">
+      <c r="J30" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K30" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+    </row>
+    <row r="31" spans="1:16" s="8" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>81</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="L28" s="6"/>
-      <c r="M28" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>73</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>80</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K30" s="6" t="s">
+      <c r="H31" s="7"/>
+      <c r="I31" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="L30" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="M30" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" ht="90" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>81</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="L31" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="J31" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K31" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+    </row>
+    <row r="32" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>85</v>
       </c>
@@ -2526,21 +2914,30 @@
         <v>112</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="I32" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K32" s="6" t="s">
+      <c r="I32" s="6" t="s">
         <v>102</v>
       </c>
+      <c r="J32" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K32" s="15" t="s">
+        <v>191</v>
+      </c>
       <c r="L32" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="M32" s="2"/>
-    </row>
-    <row r="33" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P32" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>86</v>
       </c>
@@ -2561,21 +2958,32 @@
         <v>112</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="I33" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K33" s="6" t="s">
+      <c r="I33" s="6" t="s">
         <v>102</v>
       </c>
+      <c r="J33" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K33" s="15" t="s">
+        <v>191</v>
+      </c>
       <c r="L33" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="M33" s="2"/>
-    </row>
-    <row r="34" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="O33" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>87</v>
       </c>
@@ -2596,21 +3004,30 @@
         <v>112</v>
       </c>
       <c r="H34" s="2"/>
-      <c r="I34" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K34" s="6" t="s">
+      <c r="I34" s="6" t="s">
         <v>100</v>
       </c>
+      <c r="J34" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="L34" s="6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="M34" s="2"/>
-    </row>
-    <row r="35" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N34" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>89</v>
       </c>
@@ -2631,23 +3048,28 @@
         <v>112</v>
       </c>
       <c r="H35" s="2"/>
-      <c r="I35" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K35" s="6" t="s">
+      <c r="I35" s="6" t="s">
         <v>102</v>
       </c>
+      <c r="J35" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K35" s="15" t="s">
+        <v>191</v>
+      </c>
       <c r="L35" s="6" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="M35" s="6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>90</v>
       </c>
@@ -2671,13 +3093,13 @@
         <v>113</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K36" s="2" t="s">
         <v>101</v>
+      </c>
+      <c r="J36" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K36" s="15" t="s">
+        <v>191</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>125</v>
@@ -2685,8 +3107,17 @@
       <c r="M36" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N36" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>91</v>
       </c>
@@ -2709,23 +3140,32 @@
       <c r="H37" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K37" s="5" t="s">
+      <c r="I37" s="5" t="s">
         <v>101</v>
+      </c>
+      <c r="J37" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K37" s="15" t="s">
+        <v>191</v>
       </c>
       <c r="L37" s="5" t="s">
         <v>125</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+      <c r="N37" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>92</v>
       </c>
@@ -2748,21 +3188,30 @@
       <c r="H38" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K38" s="5" t="s">
+      <c r="I38" s="5" t="s">
         <v>100</v>
+      </c>
+      <c r="J38" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K38" s="15" t="s">
+        <v>193</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>127</v>
       </c>
       <c r="M38" s="5"/>
-    </row>
-    <row r="39" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="N38" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>94</v>
       </c>
@@ -2785,14 +3234,14 @@
       <c r="H39" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K39" s="5" t="s">
+      <c r="I39" s="5" t="s">
         <v>101</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K39" s="15" t="s">
+        <v>193</v>
       </c>
       <c r="L39" s="5" t="s">
         <v>128</v>
@@ -2800,45 +3249,57 @@
       <c r="M39" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+      <c r="N39" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O39" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P39" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
         <v>95</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D40" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2" t="s">
+      <c r="F40" s="7"/>
+      <c r="G40" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="H40" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I40" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K40" s="5" t="s">
+      <c r="I40" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5" t="s">
+      <c r="J40" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K40" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+    </row>
+    <row r="41" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>99</v>
       </c>
@@ -2861,21 +3322,30 @@
       <c r="H41" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K41" s="5" t="s">
+      <c r="I41" s="5" t="s">
         <v>130</v>
+      </c>
+      <c r="J41" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K41" s="15" t="s">
+        <v>193</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>128</v>
       </c>
       <c r="M41" s="5"/>
-    </row>
-    <row r="42" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="N41" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O41" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P41" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>105</v>
       </c>
@@ -2898,21 +3368,30 @@
       <c r="H42" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K42" s="5" t="s">
+      <c r="I42" s="5" t="s">
         <v>130</v>
+      </c>
+      <c r="J42" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K42" s="15" t="s">
+        <v>193</v>
       </c>
       <c r="L42" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="M42" s="5"/>
-    </row>
-    <row r="43" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="M42" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="N42" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O42" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="P42" s="2"/>
+    </row>
+    <row r="43" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>106</v>
       </c>
@@ -2935,21 +3414,28 @@
       <c r="H43" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I43" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K43" s="5" t="s">
+      <c r="I43" s="5" t="s">
         <v>130</v>
+      </c>
+      <c r="J43" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K43" s="15" t="s">
+        <v>191</v>
       </c>
       <c r="L43" s="5"/>
       <c r="M43" s="5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O43" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="P43" s="2"/>
+    </row>
+    <row r="44" spans="1:16" ht="180" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>107</v>
       </c>
@@ -2972,23 +3458,30 @@
       <c r="H44" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I44" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K44" s="5" t="s">
+      <c r="I44" s="5" t="s">
         <v>130</v>
       </c>
+      <c r="J44" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K44" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="L44" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O44" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="P44" s="2"/>
+    </row>
+    <row r="45" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>108</v>
       </c>
@@ -3011,21 +3504,30 @@
       <c r="H45" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I45" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K45" s="5" t="s">
+      <c r="I45" s="5" t="s">
         <v>130</v>
+      </c>
+      <c r="J45" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K45" s="15" t="s">
+        <v>193</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="M45" s="5"/>
-    </row>
-    <row r="46" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+      <c r="M45" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="P45" s="2"/>
+    </row>
+    <row r="46" spans="1:16" ht="180" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>109</v>
       </c>
@@ -3048,56 +3550,66 @@
       <c r="H46" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K46" s="5" t="s">
+      <c r="I46" s="5" t="s">
         <v>130</v>
       </c>
+      <c r="J46" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K46" s="15" t="s">
+        <v>193</v>
+      </c>
       <c r="L46" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M46" s="5" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+        <v>185</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="P46" s="2"/>
+    </row>
+    <row r="47" spans="1:16" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
         <v>111</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D47" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2" t="s">
+      <c r="E47" s="7"/>
+      <c r="F47" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2" t="s">
+      <c r="G47" s="7"/>
+      <c r="H47" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5" t="s">
+      <c r="I47" s="7"/>
+      <c r="J47" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K47" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="7"/>
+    </row>
+    <row r="48" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>112</v>
       </c>
@@ -3120,21 +3632,30 @@
       <c r="H48" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K48" s="5" t="s">
+      <c r="I48" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="J48" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="K48" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L48" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="L48" s="5" t="s">
-        <v>134</v>
-      </c>
       <c r="M48" s="5"/>
-    </row>
-    <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="N48" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O48" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="P48" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>114</v>
       </c>
@@ -3157,19 +3678,28 @@
       <c r="H49" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="J49" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="K49" s="5" t="s">
+      <c r="I49" s="5" t="s">
         <v>100</v>
+      </c>
+      <c r="J49" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="K49" s="15" t="s">
+        <v>191</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>127</v>
       </c>
       <c r="M49" s="5"/>
+      <c r="N49" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>153</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Uploaded after group review
</commit_message>
<xml_diff>
--- a/data_dict_reduced.xlsx
+++ b/data_dict_reduced.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="207">
   <si>
     <t>LoanStatNew</t>
   </si>
@@ -558,15 +558,9 @@
     <t>Yes - proportion of loan amount</t>
   </si>
   <si>
-    <t>Can we delete this column? This information will not be available for new customer</t>
-  </si>
-  <si>
     <t>Yes - yearly installment proportion to annual income</t>
   </si>
   <si>
-    <t>Can we delete this column?</t>
-  </si>
-  <si>
     <t>Yes, 2</t>
   </si>
   <si>
@@ -585,10 +579,6 @@
     <t>Yes, &gt;35k</t>
   </si>
   <si>
-    <t xml:space="preserve">This data has lot of NA values - can we impute with 0?
-</t>
-  </si>
-  <si>
     <t>This data only has NA, we can delete it from our analysis - Is this right?</t>
   </si>
   <si>
@@ -601,14 +591,7 @@
     <t>Can we impute 0?</t>
   </si>
   <si>
-    <t>Values only available for charged off customers. - should we delete this column?</t>
-  </si>
-  <si>
     <t>Yes, 50</t>
-  </si>
-  <si>
-    <t>Need to remove %
-Can we impute using 0?</t>
   </si>
   <si>
     <t>Yes - proportion of total account</t>
@@ -658,6 +641,57 @@
   </si>
   <si>
     <t>use in derived metrics</t>
+  </si>
+  <si>
+    <t>rank-frequency plot
+grouped bar chart by loan status
+If possible bivariate analysis with state wise income / economic parameter.</t>
+  </si>
+  <si>
+    <t>Y, see column L</t>
+  </si>
+  <si>
+    <t>Will see later</t>
+  </si>
+  <si>
+    <t>Y - surplus amount</t>
+  </si>
+  <si>
+    <t>fillna</t>
+  </si>
+  <si>
+    <t>Can we delete this column? - Delete with high variance</t>
+  </si>
+  <si>
+    <t>Can we delete this column? This information will not be available for new customer - this can be past 6 months from decision as well.
+State the assumption</t>
+  </si>
+  <si>
+    <t>Yes - yearly installment proportion to annual income
+2. percentage of installement on dti</t>
+  </si>
+  <si>
+    <t>installment vs home ownership</t>
+  </si>
+  <si>
+    <t>Y - month and year</t>
+  </si>
+  <si>
+    <t>see current code</t>
+  </si>
+  <si>
+    <t>Will this information be available for new customer - Delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This data has lot of NA values - can we impute with 0? Fill NA
+</t>
+  </si>
+  <si>
+    <t>Values only available for charged off customers. - should we delete this column? - Delete</t>
+  </si>
+  <si>
+    <t>Need to remove %
+Can we impute using 0? - Yes</t>
   </si>
 </sst>
 </file>
@@ -800,7 +834,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1000,12 +1034,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1192,7 +1220,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1218,19 +1246,13 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1566,10 +1588,10 @@
   <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,12 +1602,13 @@
     <col min="4" max="5" width="11.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" style="1" customWidth="1"/>
-    <col min="8" max="11" width="9.140625" style="1"/>
+    <col min="8" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="16.140625" style="1" customWidth="1"/>
     <col min="12" max="12" width="43.140625" style="1" customWidth="1"/>
     <col min="13" max="13" width="24.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="10.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="11" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10" style="1" customWidth="1"/>
+    <col min="15" max="15" width="11" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="10" style="1" hidden="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1615,11 +1638,11 @@
       <c r="I1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>189</v>
+      <c r="J1" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>184</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>118</v>
@@ -1631,13 +1654,13 @@
         <v>152</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>2</v>
       </c>
@@ -1661,14 +1684,14 @@
       <c r="I2" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="J2" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>191</v>
+      <c r="J2" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>193</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>127</v>
+        <v>192</v>
       </c>
       <c r="M2" s="6"/>
       <c r="N2" s="2" t="s">
@@ -1681,7 +1704,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>4</v>
       </c>
@@ -1705,11 +1728,11 @@
       <c r="I3" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J3" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="K3" s="15" t="s">
-        <v>193</v>
+      <c r="J3" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>156</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>144</v>
@@ -1725,47 +1748,47 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:16" s="10" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+    <row r="4" spans="1:16" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
         <v>11</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="J4" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K4" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="L4" s="9" t="s">
+      <c r="J4" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="L4" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
     </row>
     <row r="5" spans="1:16" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
@@ -1793,11 +1816,11 @@
       <c r="I5" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="J5" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>191</v>
+      <c r="J5" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>186</v>
       </c>
       <c r="L5" s="7" t="s">
         <v>144</v>
@@ -1833,13 +1856,15 @@
       <c r="I6" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J6" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="L6" s="7"/>
+      <c r="J6" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>194</v>
+      </c>
       <c r="M6" s="7" t="s">
         <v>122</v>
       </c>
@@ -1871,11 +1896,11 @@
       <c r="I7" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J7" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="K7" s="15" t="s">
-        <v>193</v>
+      <c r="J7" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>195</v>
       </c>
       <c r="L7" s="6" t="s">
         <v>144</v>
@@ -1915,11 +1940,11 @@
       <c r="I8" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="J8" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K8" s="15" t="s">
-        <v>191</v>
+      <c r="J8" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L8" s="6" t="s">
         <v>147</v>
@@ -1959,17 +1984,19 @@
       <c r="I9" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="J9" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>193</v>
+      <c r="J9" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L9" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="M9" s="2"/>
-      <c r="N9" s="12" t="s">
+      <c r="M9" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="N9" s="10" t="s">
         <v>161</v>
       </c>
       <c r="O9" s="2" t="s">
@@ -1979,49 +2006,49 @@
         <v>153</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:16" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>20</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="6" t="s">
+      <c r="H10" s="7"/>
+      <c r="I10" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="J10" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="L10" s="6" t="s">
+      <c r="J10" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="L10" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="N10" s="12" t="s">
+      <c r="M10" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="N10" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="O10" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="P10" s="2" t="s">
+      <c r="P10" s="7" t="s">
         <v>153</v>
       </c>
     </row>
@@ -2049,11 +2076,11 @@
       <c r="I11" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J11" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>193</v>
+      <c r="J11" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>164</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>149</v>
@@ -2093,11 +2120,11 @@
       <c r="I12" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J12" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>191</v>
+      <c r="J12" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>164</v>
       </c>
       <c r="L12" s="6" t="s">
         <v>150</v>
@@ -2137,11 +2164,11 @@
       <c r="I13" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="J13" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>193</v>
+      <c r="J13" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L13" s="6" t="s">
         <v>151</v>
@@ -2181,11 +2208,11 @@
         <v>113</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>193</v>
+      <c r="J14" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
@@ -2223,11 +2250,11 @@
         <v>114</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="J15" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>191</v>
+      <c r="J15" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
@@ -2235,7 +2262,7 @@
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
     </row>
-    <row r="16" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>32</v>
       </c>
@@ -2259,15 +2286,15 @@
         <v>113</v>
       </c>
       <c r="I16" s="2"/>
-      <c r="J16" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>191</v>
+      <c r="J16" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="K16" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="N16" s="2" t="s">
         <v>153</v>
@@ -2275,7 +2302,7 @@
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
     </row>
-    <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="120" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>33</v>
       </c>
@@ -2299,13 +2326,15 @@
         <v>113</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="L17" s="2"/>
+      <c r="J17" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>200</v>
+      </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2" t="s">
         <v>153</v>
@@ -2314,7 +2343,7 @@
         <v>155</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.25">
@@ -2341,11 +2370,11 @@
         <v>113</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="J18" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>193</v>
+      <c r="J18" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="K18" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L18" s="2"/>
       <c r="M18" s="2" t="s">
@@ -2385,14 +2414,16 @@
         <v>113</v>
       </c>
       <c r="I19" s="2"/>
-      <c r="J19" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>191</v>
+      <c r="J19" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K19" s="13" t="s">
+        <v>201</v>
       </c>
       <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
+      <c r="M19" s="2" t="s">
+        <v>202</v>
+      </c>
       <c r="N19" s="2" t="s">
         <v>153</v>
       </c>
@@ -2403,127 +2434,127 @@
         <v>153</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="20" spans="1:16" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
         <v>36</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="5" t="s">
+      <c r="F20" s="7"/>
+      <c r="G20" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2" t="s">
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="K20" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="P20" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>39</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="O21" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="P21" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>40</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="N22" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="N20" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="O20" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>39</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K21" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="O21" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>40</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="N22" s="13" t="s">
-        <v>171</v>
-      </c>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
     </row>
     <row r="23" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -2547,11 +2578,11 @@
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-      <c r="J23" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="K23" s="15" t="s">
-        <v>193</v>
+      <c r="J23" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>170</v>
       </c>
       <c r="L23" s="2"/>
       <c r="M23" s="2"/>
@@ -2562,7 +2593,7 @@
         <v>155</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -2591,11 +2622,11 @@
       <c r="I24" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="J24" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="K24" s="15" t="s">
-        <v>193</v>
+      <c r="J24" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="L24" s="2"/>
       <c r="M24" s="2" t="s">
@@ -2631,11 +2662,11 @@
         <v>114</v>
       </c>
       <c r="I25" s="7"/>
-      <c r="J25" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K25" s="15" t="s">
-        <v>191</v>
+      <c r="J25" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
@@ -2667,11 +2698,11 @@
       <c r="I26" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="J26" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="K26" s="14" t="s">
-        <v>191</v>
+      <c r="J26" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>186</v>
       </c>
       <c r="L26" s="7" t="s">
         <v>136</v>
@@ -2707,20 +2738,20 @@
       <c r="I27" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J27" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K27" s="15" t="s">
-        <v>191</v>
+      <c r="J27" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="K27" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L27" s="6" t="s">
         <v>135</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="N27" s="13" t="s">
-        <v>173</v>
+        <v>204</v>
+      </c>
+      <c r="N27" s="11" t="s">
+        <v>171</v>
       </c>
       <c r="O27" s="2" t="s">
         <v>155</v>
@@ -2753,11 +2784,11 @@
       <c r="I28" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="J28" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K28" s="15" t="s">
-        <v>191</v>
+      <c r="J28" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L28" s="7"/>
       <c r="M28" s="7" t="s">
@@ -2767,7 +2798,7 @@
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
     </row>
-    <row r="29" spans="1:16" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="9" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>73</v>
       </c>
@@ -2791,17 +2822,17 @@
       <c r="I29" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="J29" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K29" s="15" t="s">
-        <v>193</v>
+      <c r="J29" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="L29" s="6" t="s">
         <v>139</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="N29" s="6" t="s">
         <v>153</v>
@@ -2810,7 +2841,7 @@
         <v>155</v>
       </c>
       <c r="P29" s="6" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:16" s="8" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -2837,11 +2868,11 @@
       <c r="I30" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="J30" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K30" s="15" t="s">
-        <v>193</v>
+      <c r="J30" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="K30" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="L30" s="7" t="s">
         <v>135</v>
@@ -2877,11 +2908,11 @@
       <c r="I31" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="J31" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K31" s="15" t="s">
-        <v>191</v>
+      <c r="J31" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="K31" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L31" s="7" t="s">
         <v>135</v>
@@ -2893,7 +2924,7 @@
       <c r="O31" s="7"/>
       <c r="P31" s="7"/>
     </row>
-    <row r="32" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>85</v>
       </c>
@@ -2917,11 +2948,11 @@
       <c r="I32" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J32" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K32" s="15" t="s">
-        <v>191</v>
+      <c r="J32" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L32" s="6" t="s">
         <v>141</v>
@@ -2934,10 +2965,10 @@
         <v>155</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" ht="45" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>86</v>
       </c>
@@ -2961,26 +2992,26 @@
       <c r="I33" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="J33" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K33" s="15" t="s">
-        <v>191</v>
+      <c r="J33" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L33" s="6" t="s">
         <v>141</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
+      </c>
+      <c r="N33" s="11" t="s">
+        <v>173</v>
       </c>
       <c r="O33" s="2" t="s">
         <v>155</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="45" x14ac:dyDescent="0.25">
@@ -3007,11 +3038,11 @@
       <c r="I34" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="J34" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="K34" s="15" t="s">
-        <v>193</v>
+      <c r="J34" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L34" s="6" t="s">
         <v>142</v>
@@ -3027,47 +3058,47 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+    <row r="35" spans="1:16" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
         <v>89</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2" t="s">
+      <c r="F35" s="7"/>
+      <c r="G35" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="6" t="s">
+      <c r="H35" s="7"/>
+      <c r="I35" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="J35" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K35" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="L35" s="6" t="s">
+      <c r="J35" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="L35" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="M35" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="N35" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
+      <c r="M35" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
     </row>
     <row r="36" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
@@ -3095,11 +3126,11 @@
       <c r="I36" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="J36" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K36" s="15" t="s">
-        <v>191</v>
+      <c r="J36" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K36" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>125</v>
@@ -3143,20 +3174,20 @@
       <c r="I37" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="J37" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K37" s="15" t="s">
-        <v>191</v>
+      <c r="J37" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L37" s="5" t="s">
         <v>125</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="N37" s="13" t="s">
-        <v>180</v>
+        <v>206</v>
+      </c>
+      <c r="N37" s="11" t="s">
+        <v>176</v>
       </c>
       <c r="O37" s="2" t="s">
         <v>154</v>
@@ -3191,11 +3222,11 @@
       <c r="I38" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J38" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="K38" s="15" t="s">
-        <v>193</v>
+      <c r="J38" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K38" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L38" s="5" t="s">
         <v>127</v>
@@ -3237,11 +3268,11 @@
       <c r="I39" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="J39" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="K39" s="15" t="s">
-        <v>193</v>
+      <c r="J39" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K39" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L39" s="5" t="s">
         <v>128</v>
@@ -3285,11 +3316,11 @@
       <c r="I40" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="J40" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K40" s="15" t="s">
-        <v>191</v>
+      <c r="J40" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="K40" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L40" s="7"/>
       <c r="M40" s="7" t="s">
@@ -3325,11 +3356,11 @@
       <c r="I41" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="J41" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K41" s="15" t="s">
-        <v>193</v>
+      <c r="J41" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>178</v>
       </c>
       <c r="L41" s="5" t="s">
         <v>128</v>
@@ -3342,236 +3373,236 @@
         <v>155</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>105</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2" t="s">
+      <c r="F42" s="7"/>
+      <c r="G42" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="I42" s="5" t="s">
+      <c r="I42" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="J42" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K42" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="L42" s="5" t="s">
+      <c r="J42" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="L42" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="M42" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="N42" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="O42" s="2" t="s">
+      <c r="M42" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="N42" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="O42" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="P42" s="7"/>
+    </row>
+    <row r="43" spans="1:16" s="8" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>106</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="K43" s="7" t="s">
         <v>186</v>
       </c>
-      <c r="P42" s="2"/>
-    </row>
-    <row r="43" spans="1:16" ht="135" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="L43" s="7"/>
+      <c r="M43" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="N43" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="O43" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="P43" s="7"/>
+    </row>
+    <row r="44" spans="1:16" s="8" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>107</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="H44" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="K44" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="L44" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="M44" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="N44" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="O44" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="P44" s="7"/>
+    </row>
+    <row r="45" spans="1:16" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>108</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2" t="s">
+      <c r="E45" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="H45" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="I45" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="J43" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K43" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="N43" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="O43" s="2" t="s">
+      <c r="J45" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="K45" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="L45" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="M45" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="N45" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="O45" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="P43" s="2"/>
-    </row>
-    <row r="44" spans="1:16" ht="180" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>107</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="P45" s="7"/>
+    </row>
+    <row r="46" spans="1:16" s="8" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>109</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D46" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E46" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2" t="s">
+      <c r="F46" s="7"/>
+      <c r="G46" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H46" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="I44" s="5" t="s">
+      <c r="I46" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="J44" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K44" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="L44" s="5" t="s">
+      <c r="J46" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="K46" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="L46" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="M44" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="N44" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="O44" s="2" t="s">
+      <c r="M46" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="N46" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="O46" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="P44" s="2"/>
-    </row>
-    <row r="45" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>108</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J45" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K45" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="L45" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="M45" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="N45" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="O45" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="P45" s="2"/>
-    </row>
-    <row r="46" spans="1:16" ht="180" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
-        <v>109</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J46" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K46" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="L46" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="M46" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="N46" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="O46" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="P46" s="2"/>
+      <c r="P46" s="7"/>
     </row>
     <row r="47" spans="1:16" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
@@ -3595,11 +3626,11 @@
         <v>114</v>
       </c>
       <c r="I47" s="7"/>
-      <c r="J47" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K47" s="15" t="s">
-        <v>191</v>
+      <c r="J47" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="K47" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L47" s="7"/>
       <c r="M47" s="7" t="s">
@@ -3635,11 +3666,11 @@
       <c r="I48" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="J48" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="K48" s="15" t="s">
-        <v>191</v>
+      <c r="J48" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="K48" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L48" s="5" t="s">
         <v>133</v>
@@ -3681,11 +3712,11 @@
       <c r="I49" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="J49" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="K49" s="15" t="s">
-        <v>191</v>
+      <c r="J49" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="K49" s="13" t="s">
+        <v>186</v>
       </c>
       <c r="L49" s="5" t="s">
         <v>127</v>

</xml_diff>